<commit_message>
updated roadmap for 23-05-2020
</commit_message>
<xml_diff>
--- a/roadmap + timetable.xlsx
+++ b/roadmap + timetable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hiele\Documents\School\Jaar 5 UvA 2019-20\Scriptie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hiele\Documents\School\Jaar 5 UvA 2019-20\Scriptie\Thesis\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
   <si>
     <t>Things to do</t>
   </si>
@@ -313,13 +313,34 @@
     <t>time table, github</t>
   </si>
   <si>
-    <t>Progress</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
     <t>Input physical values for the clump mass, position, velocity without any radiation. Make a animation of clumps merging on realistic timescales and lengthscales. Don't add a radiation source yet.</t>
+  </si>
+  <si>
+    <t>make 3D animation at a bad day</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>add drag of clump moving through stationary background gas</t>
+  </si>
+  <si>
+    <t>add color gradient in 3D plot</t>
+  </si>
+  <si>
+    <t>Progress legenda</t>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t>off day / weekend</t>
+  </si>
+  <si>
+    <t>paper / presentation</t>
   </si>
 </sst>
 </file>
@@ -436,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -474,6 +495,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -483,7 +609,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -518,6 +644,58 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Controlecel" xfId="5" builtinId="23"/>
@@ -806,7 +984,7 @@
   <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -854,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>35</v>
@@ -1079,462 +1257,485 @@
     <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="D15" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="21">
+        <v>43963</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="8">
-        <v>43963</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="8">
+    <row r="17" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="16">
         <v>43964</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="8">
+      <c r="F17" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="14">
         <v>43965</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="8">
+      <c r="F18" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="14">
         <v>43966</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="8">
+      <c r="F19" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="16">
         <v>43967</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="8">
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="22">
         <v>43968</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="8">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="12">
         <v>43969</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="8">
+    <row r="23" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="14">
         <v>43970</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="8">
+    <row r="24" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="14">
         <v>43971</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="8">
+    <row r="25" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="16">
         <v>43972</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="8">
+    <row r="26" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="16">
         <v>43973</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="8">
+    <row r="27" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="17">
         <v>43974</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="8">
+    <row r="28" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="19">
         <v>43975</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="8">
+    <row r="29" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="23">
         <v>43976</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="8">
+    <row r="30" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="17">
         <v>43977</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="8">
+    <row r="31" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="17">
         <v>43978</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="8">
+    <row r="32" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="17">
         <v>43979</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="8">
+      <c r="D33" s="17">
         <v>43980</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="34" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D34" s="8">
+      <c r="D34" s="17">
         <v>43981</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="8">
+    <row r="35" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="19">
         <v>43982</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="8">
+      <c r="D36" s="23">
         <v>43983</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="25" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="37" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="8">
+      <c r="D37" s="17">
         <v>43984</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="38" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="8">
+      <c r="D38" s="17">
         <v>43985</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="26" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="39" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="8">
+      <c r="D39" s="17">
         <v>43986</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="26" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="40" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="8">
+      <c r="D40" s="17">
         <v>43987</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="26" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="41" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="8">
+      <c r="D41" s="17">
         <v>43988</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="8">
+    <row r="42" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="19">
         <v>43989</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="43" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="8">
+      <c r="D43" s="23">
         <v>43990</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="25" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="44" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D44" s="8">
+      <c r="D44" s="17">
         <v>43991</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="45" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D45" s="8">
+      <c r="D45" s="17">
         <v>43992</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D46" s="8">
+      <c r="D46" s="17">
         <v>43993</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="47" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="8">
+      <c r="D47" s="17">
         <v>43994</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="26" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="48" spans="4:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D48" s="8">
+      <c r="D48" s="17">
         <v>43995</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="49" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="8">
+      <c r="D49" s="19">
         <v>43996</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="8">
+    <row r="50" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="23">
         <v>43997</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="27" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="51" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="8">
+      <c r="D51" s="17">
         <v>43998</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="52" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="8">
+      <c r="D52" s="17">
         <v>43999</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="53" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="8">
+      <c r="D53" s="17">
         <v>44000</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="54" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="8">
+      <c r="D54" s="17">
         <v>44001</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="55" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D55" s="8">
+      <c r="D55" s="17">
         <v>44002</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="56" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="8">
+      <c r="D56" s="19">
         <v>44003</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="8">
+    <row r="57" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="23">
         <v>44004</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="27" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="58" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="8">
+      <c r="D58" s="17">
         <v>44005</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="59" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="8">
+      <c r="D59" s="17">
         <v>44006</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="60" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="8">
+      <c r="D60" s="17">
         <v>44007</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="61" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="8">
+      <c r="D61" s="17">
         <v>44008</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="E61" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="62" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="8">
+      <c r="D62" s="17">
         <v>44009</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="63" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="8">
+      <c r="D63" s="19">
         <v>44010</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="4:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="8">
+    <row r="64" spans="4:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="23">
         <v>44011</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E64" s="27" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="8">
+      <c r="D65" s="17">
         <v>44012</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="66" spans="2:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="8">
+      <c r="D66" s="17">
         <v>44013</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E66" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="67" spans="2:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="8">
+      <c r="D67" s="17">
         <v>44014</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="68" spans="2:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="8">
+      <c r="D68" s="17">
         <v>44015</v>
       </c>
-      <c r="E68" s="6" t="s">
+      <c r="E68" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="69" spans="2:5" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D69" s="8">
+      <c r="D69" s="17">
         <v>44016</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="8">
+      <c r="D70" s="19">
         <v>44017</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E70" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="2:5" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="8">
         <v>44018</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="24" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>